<commit_message>
rifdid wo sltt and wo artw results
</commit_message>
<xml_diff>
--- a/linreg/rifdid_coefs-sltt-wo-ar2w.xlsx
+++ b/linreg/rifdid_coefs-sltt-wo-ar2w.xlsx
@@ -582,16 +582,16 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>-0.12254430013179642</v>
+        <v>-0.12530191092949597</v>
       </c>
       <c r="C2">
-        <v>0.0051291089512091066</v>
+        <v>0.0045755572673694964</v>
       </c>
       <c r="D2">
-        <v>-0.13259718692461808</v>
+        <v>-0.13426985608714853</v>
       </c>
       <c r="E2">
-        <v>-0.11249141333897475</v>
+        <v>-0.11633396577184341</v>
       </c>
     </row>
     <row r="3">
@@ -599,16 +599,16 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>-0.052104553465419923</v>
+        <v>-0.051397117881933706</v>
       </c>
       <c r="C3">
-        <v>0.009658823469018845</v>
+        <v>0.010625353419378973</v>
       </c>
       <c r="D3">
-        <v>-0.071035533448406227</v>
+        <v>-0.072222469020079991</v>
       </c>
       <c r="E3">
-        <v>-0.033173573482433619</v>
+        <v>-0.030571766743787424</v>
       </c>
     </row>
     <row r="4">
@@ -616,16 +616,16 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>-0.11485425006961546</v>
+        <v>-0.11991998642674441</v>
       </c>
       <c r="C4">
-        <v>0.032580227170944588</v>
+        <v>0.034251707849226293</v>
       </c>
       <c r="D4">
-        <v>-0.17871043611470022</v>
+        <v>-0.18705223275187699</v>
       </c>
       <c r="E4">
-        <v>-0.050998064024530693</v>
+        <v>-0.052787740101611844</v>
       </c>
     </row>
     <row r="5">
@@ -633,16 +633,16 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>-0.037423205846759115</v>
+        <v>-0.03841567166912585</v>
       </c>
       <c r="C5">
-        <v>0.0030371719386931418</v>
+        <v>0.0029852513993046865</v>
       </c>
       <c r="D5">
-        <v>-0.043375963998079463</v>
+        <v>-0.044266668354717299</v>
       </c>
       <c r="E5">
-        <v>-0.031470447695438768</v>
+        <v>-0.032564674983534402</v>
       </c>
     </row>
     <row r="6">
@@ -650,16 +650,16 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>-0.048248050045620161</v>
+        <v>-0.046286340874820878</v>
       </c>
       <c r="C6">
-        <v>0.0076399242536739692</v>
+        <v>0.0078051489418208015</v>
       </c>
       <c r="D6">
-        <v>-0.063222052932034506</v>
+        <v>-0.06158418165291344</v>
       </c>
       <c r="E6">
-        <v>-0.033274047159205816</v>
+        <v>-0.030988500096728315</v>
       </c>
     </row>
     <row r="7">
@@ -667,16 +667,16 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>-0.039764442768143789</v>
+        <v>-0.038225999431163872</v>
       </c>
       <c r="C7">
-        <v>0.018274159127609355</v>
+        <v>0.01715714849896334</v>
       </c>
       <c r="D7">
-        <v>-0.075581199903141286</v>
+        <v>-0.071853458420050517</v>
       </c>
       <c r="E7">
-        <v>-0.0039476856331462917</v>
+        <v>-0.0045985404422772269</v>
       </c>
     </row>
     <row r="8">
@@ -684,16 +684,16 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>-0.11839545671672819</v>
+        <v>-0.12324202766022171</v>
       </c>
       <c r="C8">
-        <v>0.0058326647332714379</v>
+        <v>0.0061069064830554165</v>
       </c>
       <c r="D8">
-        <v>-0.12982729571043988</v>
+        <v>-0.13521137488917695</v>
       </c>
       <c r="E8">
-        <v>-0.10696361772301649</v>
+        <v>-0.11127268043126648</v>
       </c>
     </row>
     <row r="9">
@@ -701,16 +701,16 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>-0.043192750726287935</v>
+        <v>-0.057881045996387798</v>
       </c>
       <c r="C9">
-        <v>0.0096105460139512839</v>
+        <v>0.012887725167342302</v>
       </c>
       <c r="D9">
-        <v>-0.062029117926760774</v>
+        <v>-0.083140587459365423</v>
       </c>
       <c r="E9">
-        <v>-0.024356383525815092</v>
+        <v>-0.032621504533410166</v>
       </c>
     </row>
     <row r="10">
@@ -718,16 +718,16 @@
         <v>13</v>
       </c>
       <c r="B10">
-        <v>-0.064521716072952179</v>
+        <v>-0.06158746877642602</v>
       </c>
       <c r="C10">
-        <v>0.03203031483331862</v>
+        <v>0.031145423380223393</v>
       </c>
       <c r="D10">
-        <v>-0.12730012334256019</v>
+        <v>-0.12263153225849843</v>
       </c>
       <c r="E10">
-        <v>-0.0017433088033441541</v>
+        <v>-0.00054340529435361468</v>
       </c>
     </row>
     <row r="11">
@@ -735,16 +735,16 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>-0.043162391848951223</v>
+        <v>-0.045010075061445491</v>
       </c>
       <c r="C11">
-        <v>0.0034170911964450197</v>
+        <v>0.0032940567129078639</v>
       </c>
       <c r="D11">
-        <v>-0.049859781964715702</v>
+        <v>-0.051466323043159276</v>
       </c>
       <c r="E11">
-        <v>-0.036465001733186744</v>
+        <v>-0.038553827079731706</v>
       </c>
     </row>
     <row r="12">
@@ -752,16 +752,16 @@
         <v>15</v>
       </c>
       <c r="B12">
-        <v>-0.043650668978191323</v>
+        <v>-0.044491104006508533</v>
       </c>
       <c r="C12">
-        <v>0.0076508686030033078</v>
+        <v>0.0082135221375137842</v>
       </c>
       <c r="D12">
-        <v>-0.058646128219102339</v>
+        <v>-0.060589350134236358</v>
       </c>
       <c r="E12">
-        <v>-0.028655209737280304</v>
+        <v>-0.028392857878780712</v>
       </c>
     </row>
     <row r="13">
@@ -769,16 +769,16 @@
         <v>16</v>
       </c>
       <c r="B13">
-        <v>-0.020945603162291666</v>
+        <v>-0.01687596193721989</v>
       </c>
       <c r="C13">
-        <v>0.018370980984348851</v>
+        <v>0.021481316199992814</v>
       </c>
       <c r="D13">
-        <v>-0.0569521418784599</v>
+        <v>-0.058978668857019786</v>
       </c>
       <c r="E13">
-        <v>0.015060935553876567</v>
+        <v>0.025226744982580002</v>
       </c>
     </row>
     <row r="14">
@@ -786,16 +786,16 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>-0.23385990936326398</v>
+        <v>-0.23630722077625002</v>
       </c>
       <c r="C14">
-        <v>0.010015070144916075</v>
+        <v>0.010928593704329156</v>
       </c>
       <c r="D14">
-        <v>-0.25348924756700592</v>
+        <v>-0.25772706092987174</v>
       </c>
       <c r="E14">
-        <v>-0.21423057115952207</v>
+        <v>-0.21488738062262827</v>
       </c>
     </row>
     <row r="15">
@@ -803,16 +803,16 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>-0.042917966373019381</v>
+        <v>-0.043724005397899814</v>
       </c>
       <c r="C15">
-        <v>0.024746587212610055</v>
+        <v>0.026843620273929586</v>
       </c>
       <c r="D15">
-        <v>-0.091420784901085544</v>
+        <v>-0.096337001266189964</v>
       </c>
       <c r="E15">
-        <v>0.0055848521550467753</v>
+        <v>0.0088889904703903372</v>
       </c>
     </row>
     <row r="16">
@@ -820,16 +820,16 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>-0.040245954778860768</v>
+        <v>-0.038043145744966284</v>
       </c>
       <c r="C16">
-        <v>0.077745596144128973</v>
+        <v>0.074142326334681569</v>
       </c>
       <c r="D16">
-        <v>-0.19262577623616012</v>
+        <v>-0.18336072471923417</v>
       </c>
       <c r="E16">
-        <v>0.1121338666784386</v>
+        <v>0.10727443322930161</v>
       </c>
     </row>
     <row r="17">
@@ -837,16 +837,16 @@
         <v>20</v>
       </c>
       <c r="B17">
-        <v>-0.056118374985069365</v>
+        <v>-0.05695811493598249</v>
       </c>
       <c r="C17">
-        <v>0.0083502386069209608</v>
+        <v>0.0087234655535838746</v>
       </c>
       <c r="D17">
-        <v>-0.072484705564639859</v>
+        <v>-0.07405597903856373</v>
       </c>
       <c r="E17">
-        <v>-0.039752044405498871</v>
+        <v>-0.039860250833401244</v>
       </c>
     </row>
     <row r="18">
@@ -854,16 +854,16 @@
         <v>21</v>
       </c>
       <c r="B18">
-        <v>0.03665758372620103</v>
+        <v>0.036782112748222122</v>
       </c>
       <c r="C18">
-        <v>0.026648125336030153</v>
+        <v>0.024522931088801346</v>
       </c>
       <c r="D18">
-        <v>-0.015572304436972731</v>
+        <v>-0.011282471284098927</v>
       </c>
       <c r="E18">
-        <v>0.088887471889374792</v>
+        <v>0.084846696780543171</v>
       </c>
     </row>
     <row r="19">
@@ -871,16 +871,16 @@
         <v>22</v>
       </c>
       <c r="B19">
-        <v>-0.033087722537498802</v>
+        <v>-0.035960517610843609</v>
       </c>
       <c r="C19">
-        <v>0.069517451552120843</v>
+        <v>0.067065620867703402</v>
       </c>
       <c r="D19">
-        <v>-0.16934078627729229</v>
+        <v>-0.16740814751294575</v>
       </c>
       <c r="E19">
-        <v>0.10316534120229467</v>
+        <v>0.095487112291258544</v>
       </c>
     </row>
     <row r="20">
@@ -888,16 +888,16 @@
         <v>23</v>
       </c>
       <c r="B20">
-        <v>-0.17961264581406447</v>
+        <v>-0.18264053442557462</v>
       </c>
       <c r="C20">
-        <v>0.0048704934284688204</v>
+        <v>0.0048233177637033407</v>
       </c>
       <c r="D20">
-        <v>-0.18915865459011841</v>
+        <v>-0.19209408219150403</v>
       </c>
       <c r="E20">
-        <v>-0.17006663703801053</v>
+        <v>-0.17318698665964521</v>
       </c>
     </row>
     <row r="21">
@@ -905,16 +905,16 @@
         <v>24</v>
       </c>
       <c r="B21">
-        <v>-0.022705687381255186</v>
+        <v>-0.018117452426962929</v>
       </c>
       <c r="C21">
-        <v>0.0093681843837608494</v>
+        <v>0.0098333954838038806</v>
       </c>
       <c r="D21">
-        <v>-0.041067024206051385</v>
+        <v>-0.037390591469753168</v>
       </c>
       <c r="E21">
-        <v>-0.0043443505564589868</v>
+        <v>0.0011556866158273123</v>
       </c>
     </row>
     <row r="22">
@@ -922,16 +922,16 @@
         <v>25</v>
       </c>
       <c r="B22">
-        <v>-0.13899384139049206</v>
+        <v>-0.13649877216343909</v>
       </c>
       <c r="C22">
-        <v>0.028001211368866342</v>
+        <v>0.029992212123779744</v>
       </c>
       <c r="D22">
-        <v>-0.1938753053310712</v>
+        <v>-0.19528254379293727</v>
       </c>
       <c r="E22">
-        <v>-0.084112377449912928</v>
+        <v>-0.077715000533940898</v>
       </c>
     </row>
     <row r="23">
@@ -939,16 +939,16 @@
         <v>26</v>
       </c>
       <c r="B23">
-        <v>-0.061855925730089953</v>
+        <v>-0.063875378169299071</v>
       </c>
       <c r="C23">
-        <v>0.0030918085362498658</v>
+        <v>0.003182547154131187</v>
       </c>
       <c r="D23">
-        <v>-0.067915769834405823</v>
+        <v>-0.07011306818592454</v>
       </c>
       <c r="E23">
-        <v>-0.055796081625774083</v>
+        <v>-0.057637688152673595</v>
       </c>
     </row>
     <row r="24">
@@ -956,16 +956,16 @@
         <v>27</v>
       </c>
       <c r="B24">
-        <v>-0.07530444895480938</v>
+        <v>-0.074905255169748844</v>
       </c>
       <c r="C24">
-        <v>0.0075665630636902684</v>
+        <v>0.0082181295746740959</v>
       </c>
       <c r="D24">
-        <v>-0.090134666296486365</v>
+        <v>-0.091012524699671443</v>
       </c>
       <c r="E24">
-        <v>-0.060474231613132402</v>
+        <v>-0.058797985639826238</v>
       </c>
     </row>
     <row r="25">
@@ -973,16 +973,16 @@
         <v>28</v>
       </c>
       <c r="B25">
-        <v>-0.075966650496434404</v>
+        <v>-0.076743616400808137</v>
       </c>
       <c r="C25">
-        <v>0.018617942106941114</v>
+        <v>0.021594917437652753</v>
       </c>
       <c r="D25">
-        <v>-0.11245721108207976</v>
+        <v>-0.11906895971452591</v>
       </c>
       <c r="E25">
-        <v>-0.03947608991078904</v>
+        <v>-0.034418273087090362</v>
       </c>
     </row>
     <row r="26">
@@ -990,16 +990,16 @@
         <v>29</v>
       </c>
       <c r="B26">
-        <v>-0.18078714666763807</v>
+        <v>-0.18504997332516049</v>
       </c>
       <c r="C26">
-        <v>0.0057697621767067555</v>
+        <v>0.0055278075169924558</v>
       </c>
       <c r="D26">
-        <v>-0.19209569863358039</v>
+        <v>-0.1958843045482265</v>
       </c>
       <c r="E26">
-        <v>-0.16947859470169574</v>
+        <v>-0.17421564210209448</v>
       </c>
     </row>
     <row r="27">
@@ -1007,16 +1007,16 @@
         <v>30</v>
       </c>
       <c r="B27">
-        <v>-0.033093861907720831</v>
+        <v>-0.02113878985032875</v>
       </c>
       <c r="C27">
-        <v>0.0097597757253193741</v>
+        <v>0.0093015318160601778</v>
       </c>
       <c r="D27">
-        <v>-0.052222714637784745</v>
+        <v>-0.039369503612936819</v>
       </c>
       <c r="E27">
-        <v>-0.013965009177656914</v>
+        <v>-0.0029080760877206804</v>
       </c>
     </row>
     <row r="28">
@@ -1024,16 +1024,16 @@
         <v>31</v>
       </c>
       <c r="B28">
-        <v>-0.11285016431721918</v>
+        <v>-0.11154155937875466</v>
       </c>
       <c r="C28">
-        <v>0.03051076122951149</v>
+        <v>0.03101471405280213</v>
       </c>
       <c r="D28">
-        <v>-0.17265029442957078</v>
+        <v>-0.17232943663457501</v>
       </c>
       <c r="E28">
-        <v>-0.053050034204867591</v>
+        <v>-0.050753682122934338</v>
       </c>
     </row>
     <row r="29">
@@ -1041,16 +1041,16 @@
         <v>32</v>
       </c>
       <c r="B29">
-        <v>-0.068317346775797649</v>
+        <v>-0.070164192669033287</v>
       </c>
       <c r="C29">
-        <v>0.0033835869362783739</v>
+        <v>0.0035841115820346753</v>
       </c>
       <c r="D29">
-        <v>-0.074949069606735336</v>
+        <v>-0.077188939109212623</v>
       </c>
       <c r="E29">
-        <v>-0.061685623944859963</v>
+        <v>-0.063139446228853952</v>
       </c>
     </row>
     <row r="30">
@@ -1058,16 +1058,16 @@
         <v>33</v>
       </c>
       <c r="B30">
-        <v>-0.085454750906393512</v>
+        <v>-0.088642480456228204</v>
       </c>
       <c r="C30">
-        <v>0.0074348171817519649</v>
+        <v>0.0073010895851059335</v>
       </c>
       <c r="D30">
-        <v>-0.1000267562299227</v>
+        <v>-0.10295238736021117</v>
       </c>
       <c r="E30">
-        <v>-0.070882745582864323</v>
+        <v>-0.074332573552245235</v>
       </c>
     </row>
     <row r="31">
@@ -1075,16 +1075,16 @@
         <v>34</v>
       </c>
       <c r="B31">
-        <v>-0.070752925138102232</v>
+        <v>-0.067232652821325123</v>
       </c>
       <c r="C31">
-        <v>0.018625874317580414</v>
+        <v>0.016650059472910466</v>
       </c>
       <c r="D31">
-        <v>-0.10725904668434985</v>
+        <v>-0.099866247879407344</v>
       </c>
       <c r="E31">
-        <v>-0.03424680359185462</v>
+        <v>-0.034599057763242895</v>
       </c>
     </row>
     <row r="32">
@@ -1092,16 +1092,16 @@
         <v>35</v>
       </c>
       <c r="B32">
-        <v>-0.17665713090381602</v>
+        <v>-0.1767814466624506</v>
       </c>
       <c r="C32">
-        <v>0.0065417154614724115</v>
+        <v>0.0081287412309863222</v>
       </c>
       <c r="D32">
-        <v>-0.18947876304096822</v>
+        <v>-0.19271362810578752</v>
       </c>
       <c r="E32">
-        <v>-0.16383549876666381</v>
+        <v>-0.16084926521911369</v>
       </c>
     </row>
     <row r="33">
@@ -1109,16 +1109,16 @@
         <v>36</v>
       </c>
       <c r="B33">
-        <v>-0.035697583517181143</v>
+        <v>-0.041831686300413486</v>
       </c>
       <c r="C33">
-        <v>0.018263168893887981</v>
+        <v>0.018409460185893112</v>
       </c>
       <c r="D33">
-        <v>-0.071493031147886715</v>
+        <v>-0.077913885452907242</v>
       </c>
       <c r="E33">
-        <v>9.7864113524429031e-05</v>
+        <v>-0.0057494871479197296</v>
       </c>
     </row>
     <row r="34">
@@ -1126,16 +1126,16 @@
         <v>37</v>
       </c>
       <c r="B34">
-        <v>-0.0042172027908380086</v>
+        <v>0.0021838262228999713</v>
       </c>
       <c r="C34">
-        <v>0.049320621796795305</v>
+        <v>0.052222293287971809</v>
       </c>
       <c r="D34">
-        <v>-0.10088464012871727</v>
+        <v>-0.10017089616382396</v>
       </c>
       <c r="E34">
-        <v>0.092450234547041252</v>
+        <v>0.10453854860962392</v>
       </c>
     </row>
     <row r="35">
@@ -1143,16 +1143,16 @@
         <v>38</v>
       </c>
       <c r="B35">
-        <v>-0.049559289817721973</v>
+        <v>-0.051497908712961976</v>
       </c>
       <c r="C35">
-        <v>0.0061695962682127214</v>
+        <v>0.0066516790944957998</v>
       </c>
       <c r="D35">
-        <v>-0.061651597214107449</v>
+        <v>-0.064535101846022055</v>
       </c>
       <c r="E35">
-        <v>-0.037466982421336496</v>
+        <v>-0.038460715579901897</v>
       </c>
     </row>
     <row r="36">
@@ -1160,16 +1160,16 @@
         <v>39</v>
       </c>
       <c r="B36">
-        <v>0.00775921868202409</v>
+        <v>0.0018390097271099967</v>
       </c>
       <c r="C36">
-        <v>0.020922736527345179</v>
+        <v>0.020585214740249429</v>
       </c>
       <c r="D36">
-        <v>-0.033249001412665152</v>
+        <v>-0.038507708213059946</v>
       </c>
       <c r="E36">
-        <v>0.048767438776713329</v>
+        <v>0.042185727667279946</v>
       </c>
     </row>
     <row r="37">
@@ -1177,16 +1177,16 @@
         <v>40</v>
       </c>
       <c r="B37">
-        <v>-0.070485674982321583</v>
+        <v>-0.079175390338009466</v>
       </c>
       <c r="C37">
-        <v>0.047025692369547539</v>
+        <v>0.046317142881061923</v>
       </c>
       <c r="D37">
-        <v>-0.16265525998259917</v>
+        <v>-0.16995630873974349</v>
       </c>
       <c r="E37">
-        <v>0.021683910017955998</v>
+        <v>0.011605528063724557</v>
       </c>
     </row>
     <row r="38">
@@ -1194,16 +1194,16 @@
         <v>41</v>
       </c>
       <c r="B38">
-        <v>-0.18850148430430025</v>
+        <v>-0.18878584661722111</v>
       </c>
       <c r="C38">
-        <v>0.0042324489729324948</v>
+        <v>0.0045887807441638622</v>
       </c>
       <c r="D38">
-        <v>-0.19679694669085271</v>
+        <v>-0.19777970936430722</v>
       </c>
       <c r="E38">
-        <v>-0.18020602191774779</v>
+        <v>-0.17979198387013501</v>
       </c>
     </row>
     <row r="39">
@@ -1211,16 +1211,16 @@
         <v>42</v>
       </c>
       <c r="B39">
-        <v>-0.01449045980132694</v>
+        <v>-0.014601094043066393</v>
       </c>
       <c r="C39">
-        <v>0.008588503238627955</v>
+        <v>0.0087105275814949434</v>
       </c>
       <c r="D39">
-        <v>-0.031323646929737603</v>
+        <v>-0.031673448093172213</v>
       </c>
       <c r="E39">
-        <v>0.002342727327083724</v>
+        <v>0.002471260007039424</v>
       </c>
     </row>
     <row r="40">
@@ -1228,16 +1228,16 @@
         <v>43</v>
       </c>
       <c r="B40">
-        <v>-0.074815018718009108</v>
+        <v>-0.06788384401740355</v>
       </c>
       <c r="C40">
-        <v>0.022813805086274692</v>
+        <v>0.024867601534961981</v>
       </c>
       <c r="D40">
-        <v>-0.11952933499155095</v>
+        <v>-0.11662354362914196</v>
       </c>
       <c r="E40">
-        <v>-0.030100702444467262</v>
+        <v>-0.019144144405665135</v>
       </c>
     </row>
     <row r="41">
@@ -1245,16 +1245,16 @@
         <v>44</v>
       </c>
       <c r="B41">
-        <v>-0.074404250850460749</v>
+        <v>-0.076043219580110955</v>
       </c>
       <c r="C41">
-        <v>0.0030444915338689758</v>
+        <v>0.0030917019014280235</v>
       </c>
       <c r="D41">
-        <v>-0.080371355170100453</v>
+        <v>-0.082102855824584528</v>
       </c>
       <c r="E41">
-        <v>-0.068437146530821044</v>
+        <v>-0.069983583335637381</v>
       </c>
     </row>
     <row r="42">
@@ -1262,16 +1262,16 @@
         <v>45</v>
       </c>
       <c r="B42">
-        <v>-0.0636851247801518</v>
+        <v>-0.0699636325842493</v>
       </c>
       <c r="C42">
-        <v>0.0073886790648544894</v>
+        <v>0.0077402722232919963</v>
       </c>
       <c r="D42">
-        <v>-0.07816669527356547</v>
+        <v>-0.085134317081576871</v>
       </c>
       <c r="E42">
-        <v>-0.049203554286738137</v>
+        <v>-0.054792948086921735</v>
       </c>
     </row>
     <row r="43">
@@ -1279,16 +1279,16 @@
         <v>46</v>
       </c>
       <c r="B43">
-        <v>-0.058879679584109335</v>
+        <v>-0.059043420335350053</v>
       </c>
       <c r="C43">
-        <v>0.016955507681327104</v>
+        <v>0.015701878854959404</v>
       </c>
       <c r="D43">
-        <v>-0.092111922801536322</v>
+        <v>-0.089818597648498394</v>
       </c>
       <c r="E43">
-        <v>-0.025647436366682354</v>
+        <v>-0.028268243022201711</v>
       </c>
     </row>
     <row r="44">
@@ -1296,16 +1296,16 @@
         <v>47</v>
       </c>
       <c r="B44">
-        <v>-0.20021659353425922</v>
+        <v>-0.20422549125455597</v>
       </c>
       <c r="C44">
-        <v>0.0050319227736089827</v>
+        <v>0.0055256973606076579</v>
       </c>
       <c r="D44">
-        <v>-0.21007900353162329</v>
+        <v>-0.2150556866365792</v>
       </c>
       <c r="E44">
-        <v>-0.19035418353689515</v>
+        <v>-0.19339529587253274</v>
       </c>
     </row>
     <row r="45">
@@ -1313,16 +1313,16 @@
         <v>48</v>
       </c>
       <c r="B45">
-        <v>-0.023581095594510201</v>
+        <v>-0.024135928102501945</v>
       </c>
       <c r="C45">
-        <v>0.0090092398080205017</v>
+        <v>0.0088376571447730222</v>
       </c>
       <c r="D45">
-        <v>-0.041238921588438365</v>
+        <v>-0.041457461901938955</v>
       </c>
       <c r="E45">
-        <v>-0.0059232696005820408</v>
+        <v>-0.0068143943030649391</v>
       </c>
     </row>
     <row r="46">
@@ -1330,16 +1330,16 @@
         <v>49</v>
       </c>
       <c r="B46">
-        <v>-0.09931269423285953</v>
+        <v>-0.094524575002276637</v>
       </c>
       <c r="C46">
-        <v>0.025042223858917106</v>
+        <v>0.024399830914101545</v>
       </c>
       <c r="D46">
-        <v>-0.14839466350268543</v>
+        <v>-0.1423474865449729</v>
       </c>
       <c r="E46">
-        <v>-0.050230724963033636</v>
+        <v>-0.046701663459580371</v>
       </c>
     </row>
     <row r="47">
@@ -1347,16 +1347,16 @@
         <v>50</v>
       </c>
       <c r="B47">
-        <v>-0.090123712707175688</v>
+        <v>-0.092718146920455838</v>
       </c>
       <c r="C47">
-        <v>0.0034098027909753663</v>
+        <v>0.0032790655439740167</v>
       </c>
       <c r="D47">
-        <v>-0.096806817779917925</v>
+        <v>-0.099145012680608768</v>
       </c>
       <c r="E47">
-        <v>-0.08344060763443345</v>
+        <v>-0.086291281160302907</v>
       </c>
     </row>
     <row r="48">
@@ -1364,16 +1364,16 @@
         <v>51</v>
       </c>
       <c r="B48">
-        <v>-0.067102025361911719</v>
+        <v>-0.072701480132404087</v>
       </c>
       <c r="C48">
-        <v>0.0074934928223239832</v>
+        <v>0.0077250953680392869</v>
       </c>
       <c r="D48">
-        <v>-0.0817890330756645</v>
+        <v>-0.087842425090337836</v>
       </c>
       <c r="E48">
-        <v>-0.052415017648158937</v>
+        <v>-0.057560535174470337</v>
       </c>
     </row>
     <row r="49">
@@ -1381,16 +1381,16 @@
         <v>52</v>
       </c>
       <c r="B49">
-        <v>-0.068155508496912681</v>
+        <v>-0.064567053363305149</v>
       </c>
       <c r="C49">
-        <v>0.017580090835460666</v>
+        <v>0.016376882713585828</v>
       </c>
       <c r="D49">
-        <v>-0.1026119276636437</v>
+        <v>-0.096665230529482338</v>
       </c>
       <c r="E49">
-        <v>-0.033699089330181661</v>
+        <v>-0.032468876197127967</v>
       </c>
     </row>
     <row r="50">
@@ -1398,16 +1398,16 @@
         <v>53</v>
       </c>
       <c r="B50">
-        <v>-0.15153415065612746</v>
+        <v>-0.15204637525816525</v>
       </c>
       <c r="C50">
-        <v>0.0055537001144539411</v>
+        <v>0.0055167080910860289</v>
       </c>
       <c r="D50">
-        <v>-0.16241929237269506</v>
+        <v>-0.162859020387286</v>
       </c>
       <c r="E50">
-        <v>-0.14064900893955987</v>
+        <v>-0.1412337301290445</v>
       </c>
     </row>
     <row r="51">
@@ -1415,16 +1415,16 @@
         <v>54</v>
       </c>
       <c r="B51">
-        <v>-0.02690676095856261</v>
+        <v>-0.02880004014997704</v>
       </c>
       <c r="C51">
-        <v>0.016290695966719303</v>
+        <v>0.017584061952153739</v>
       </c>
       <c r="D51">
-        <v>-0.058836200900368146</v>
+        <v>-0.063264474134499052</v>
       </c>
       <c r="E51">
-        <v>0.0050226789832429238</v>
+        <v>0.0056643938345449681</v>
       </c>
     </row>
     <row r="52">
@@ -1432,16 +1432,16 @@
         <v>55</v>
       </c>
       <c r="B52">
-        <v>-0.010233008251776596</v>
+        <v>-0.01067311589710152</v>
       </c>
       <c r="C52">
-        <v>0.040081712534426016</v>
+        <v>0.034531888820888569</v>
       </c>
       <c r="D52">
-        <v>-0.088792367271623263</v>
+        <v>-0.078354974950299319</v>
       </c>
       <c r="E52">
-        <v>0.06832635076807006</v>
+        <v>0.057008743156096282</v>
       </c>
     </row>
     <row r="53">
@@ -1449,16 +1449,16 @@
         <v>56</v>
       </c>
       <c r="B53">
-        <v>-0.050405974443790962</v>
+        <v>-0.051509599129640121</v>
       </c>
       <c r="C53">
-        <v>0.0056673551282508533</v>
+        <v>0.0057148432319160556</v>
       </c>
       <c r="D53">
-        <v>-0.06151389745139222</v>
+        <v>-0.062710607759371442</v>
       </c>
       <c r="E53">
-        <v>-0.039298051436189703</v>
+        <v>-0.0403085904999088</v>
       </c>
     </row>
     <row r="54">
@@ -1466,16 +1466,16 @@
         <v>57</v>
       </c>
       <c r="B54">
-        <v>-0.027104970301256914</v>
+        <v>-0.029795428373610891</v>
       </c>
       <c r="C54">
-        <v>0.019514238129985751</v>
+        <v>0.021977753237612571</v>
       </c>
       <c r="D54">
-        <v>-0.065352556661136069</v>
+        <v>-0.072871501274751144</v>
       </c>
       <c r="E54">
-        <v>0.011142616058622233</v>
+        <v>0.013280644527529355</v>
       </c>
     </row>
     <row r="55">
@@ -1483,16 +1483,16 @@
         <v>58</v>
       </c>
       <c r="B55">
-        <v>-0.0005842958874392772</v>
+        <v>0.0022021018825166589</v>
       </c>
       <c r="C55">
-        <v>0.042255123048200324</v>
+        <v>0.043372044088347432</v>
       </c>
       <c r="D55">
-        <v>-0.083403643338670869</v>
+        <v>-0.082806466228246015</v>
       </c>
       <c r="E55">
-        <v>0.082235051563792322</v>
+        <v>0.087210669993279324</v>
       </c>
     </row>
     <row r="56">
@@ -1500,16 +1500,16 @@
         <v>59</v>
       </c>
       <c r="B56">
-        <v>-0.17286526192849849</v>
+        <v>-0.17510107607444475</v>
       </c>
       <c r="C56">
-        <v>0.0037069872373821878</v>
+        <v>0.0035364148201868502</v>
       </c>
       <c r="D56">
-        <v>-0.1801308363965653</v>
+        <v>-0.18203233544001229</v>
       </c>
       <c r="E56">
-        <v>-0.16559968746043169</v>
+        <v>-0.16816981670887721</v>
       </c>
     </row>
     <row r="57">
@@ -1517,16 +1517,16 @@
         <v>60</v>
       </c>
       <c r="B57">
-        <v>-0.0103552917603238</v>
+        <v>-0.022949622763375407</v>
       </c>
       <c r="C57">
-        <v>0.0078278939098947176</v>
+        <v>0.0076925102495712981</v>
       </c>
       <c r="D57">
-        <v>-0.025697709332451822</v>
+        <v>-0.038026695568213448</v>
       </c>
       <c r="E57">
-        <v>0.004987125811804223</v>
+        <v>-0.0078725499585373688</v>
       </c>
     </row>
     <row r="58">
@@ -1534,16 +1534,16 @@
         <v>61</v>
       </c>
       <c r="B58">
-        <v>-0.047463975488005808</v>
+        <v>-0.044298948580763428</v>
       </c>
       <c r="C58">
-        <v>0.018879910322760471</v>
+        <v>0.020311031063918926</v>
       </c>
       <c r="D58">
-        <v>-0.084467985919212257</v>
+        <v>-0.084107916545297354</v>
       </c>
       <c r="E58">
-        <v>-0.010459965056799365</v>
+        <v>-0.0044899806162295025</v>
       </c>
     </row>
     <row r="59">
@@ -1551,16 +1551,16 @@
         <v>62</v>
       </c>
       <c r="B59">
-        <v>-0.081916191025478063</v>
+        <v>-0.083025097686312221</v>
       </c>
       <c r="C59">
-        <v>0.0028786922322286785</v>
+        <v>0.0028660971810791397</v>
       </c>
       <c r="D59">
-        <v>-0.087558334110046182</v>
+        <v>-0.088642555938231282</v>
       </c>
       <c r="E59">
-        <v>-0.076274047940909945</v>
+        <v>-0.077407639434393161</v>
       </c>
     </row>
     <row r="60">
@@ -1568,16 +1568,16 @@
         <v>63</v>
       </c>
       <c r="B60">
-        <v>-0.061653133600517253</v>
+        <v>-0.068351067743970553</v>
       </c>
       <c r="C60">
-        <v>0.0070052773912674558</v>
+        <v>0.0073347966699881329</v>
       </c>
       <c r="D60">
-        <v>-0.075383249291982132</v>
+        <v>-0.082727033203892478</v>
       </c>
       <c r="E60">
-        <v>-0.04792301790905238</v>
+        <v>-0.053975102284048629</v>
       </c>
     </row>
     <row r="61">
@@ -1585,16 +1585,16 @@
         <v>64</v>
       </c>
       <c r="B61">
-        <v>-0.045392983397188724</v>
+        <v>-0.048023877211236889</v>
       </c>
       <c r="C61">
-        <v>0.015149626408643906</v>
+        <v>0.016742693705128209</v>
       </c>
       <c r="D61">
-        <v>-0.075085758094796812</v>
+        <v>-0.080839018140203472</v>
       </c>
       <c r="E61">
-        <v>-0.01570020869958063</v>
+        <v>-0.015208736282270312</v>
       </c>
     </row>
     <row r="62">
@@ -1602,16 +1602,16 @@
         <v>65</v>
       </c>
       <c r="B62">
-        <v>-0.20059992086975978</v>
+        <v>-0.20330057722197595</v>
       </c>
       <c r="C62">
-        <v>0.0045879121064610695</v>
+        <v>0.0052968457025804388</v>
       </c>
       <c r="D62">
-        <v>-0.20959208395761592</v>
+        <v>-0.21368223045480297</v>
       </c>
       <c r="E62">
-        <v>-0.19160775778190364</v>
+        <v>-0.19291892398914892</v>
       </c>
     </row>
     <row r="63">
@@ -1619,16 +1619,16 @@
         <v>66</v>
       </c>
       <c r="B63">
-        <v>-0.027025348936496833</v>
+        <v>-0.027298862789963848</v>
       </c>
       <c r="C63">
-        <v>0.0086980557816216057</v>
+        <v>0.0097157000650860796</v>
       </c>
       <c r="D63">
-        <v>-0.044073264049226131</v>
+        <v>-0.046341333470342694</v>
       </c>
       <c r="E63">
-        <v>-0.0099774338237675342</v>
+        <v>-0.0082563921095850056</v>
       </c>
     </row>
     <row r="64">
@@ -1636,16 +1636,16 @@
         <v>67</v>
       </c>
       <c r="B64">
-        <v>-0.038476082513537596</v>
+        <v>-0.035645306214710182</v>
       </c>
       <c r="C64">
-        <v>0.021653320455277673</v>
+        <v>0.023213003179783611</v>
       </c>
       <c r="D64">
-        <v>-0.080915907952490818</v>
+        <v>-0.081142072221623118</v>
       </c>
       <c r="E64">
-        <v>0.0039637429254156184</v>
+        <v>0.0098514597922027616</v>
       </c>
     </row>
     <row r="65">
@@ -1653,16 +1653,16 @@
         <v>68</v>
       </c>
       <c r="B65">
-        <v>-0.10492384592570865</v>
+        <v>-0.10573100737168814</v>
       </c>
       <c r="C65">
-        <v>0.0033417288679124936</v>
+        <v>0.0032576608965309639</v>
       </c>
       <c r="D65">
-        <v>-0.11147352827331646</v>
+        <v>-0.11211592069328347</v>
       </c>
       <c r="E65">
-        <v>-0.098374163578100846</v>
+        <v>-0.099346094050092815</v>
       </c>
     </row>
     <row r="66">
@@ -1670,16 +1670,16 @@
         <v>69</v>
       </c>
       <c r="B66">
-        <v>-0.067862304234621654</v>
+        <v>-0.074346702235088019</v>
       </c>
       <c r="C66">
-        <v>0.0074274983797574801</v>
+        <v>0.0077462293349204094</v>
       </c>
       <c r="D66">
-        <v>-0.082419964938906243</v>
+        <v>-0.08952906910615617</v>
       </c>
       <c r="E66">
-        <v>-0.053304643530337072</v>
+        <v>-0.059164335364019868</v>
       </c>
     </row>
     <row r="67">
@@ -1687,16 +1687,16 @@
         <v>70</v>
       </c>
       <c r="B67">
-        <v>-0.038883293440465955</v>
+        <v>-0.048623442849189492</v>
       </c>
       <c r="C67">
-        <v>0.016210399215326125</v>
+        <v>0.015388834019117795</v>
       </c>
       <c r="D67">
-        <v>-0.070655160574205275</v>
+        <v>-0.078785075521612957</v>
       </c>
       <c r="E67">
-        <v>-0.0071114263067266342</v>
+        <v>-0.018461810176766028</v>
       </c>
     </row>
     <row r="68">
@@ -1704,16 +1704,16 @@
         <v>71</v>
       </c>
       <c r="B68">
-        <v>-0.13287584335289249</v>
+        <v>-0.13269244175349526</v>
       </c>
       <c r="C68">
-        <v>0.0049455339482777812</v>
+        <v>0.0051297684733690044</v>
       </c>
       <c r="D68">
-        <v>-0.14256899148507116</v>
+        <v>-0.14274669243728871</v>
       </c>
       <c r="E68">
-        <v>-0.12318269522071382</v>
+        <v>-0.12263819106970181</v>
       </c>
     </row>
     <row r="69">
@@ -1721,16 +1721,16 @@
         <v>72</v>
       </c>
       <c r="B69">
-        <v>-0.028360027248514458</v>
+        <v>-0.031702535995972905</v>
       </c>
       <c r="C69">
-        <v>0.01471834036171729</v>
+        <v>0.014271942423673854</v>
       </c>
       <c r="D69">
-        <v>-0.057207681491315047</v>
+        <v>-0.059675277381325026</v>
       </c>
       <c r="E69">
-        <v>0.00048762699428613054</v>
+        <v>-0.0037297946106207847</v>
       </c>
     </row>
     <row r="70">
@@ -1738,16 +1738,16 @@
         <v>73</v>
       </c>
       <c r="B70">
-        <v>-0.022213797775395124</v>
+        <v>-0.022226160314343772</v>
       </c>
       <c r="C70">
-        <v>0.034627779581783952</v>
+        <v>0.035299364247715341</v>
       </c>
       <c r="D70">
-        <v>-0.090083556730654213</v>
+        <v>-0.091412256912574472</v>
       </c>
       <c r="E70">
-        <v>0.045655961179863973</v>
+        <v>0.046959936283886936</v>
       </c>
     </row>
     <row r="71">
@@ -1755,16 +1755,16 @@
         <v>74</v>
       </c>
       <c r="B71">
-        <v>-0.047676865846169425</v>
+        <v>-0.046798368907118623</v>
       </c>
       <c r="C71">
-        <v>0.0053311453237208121</v>
+        <v>0.0054510384415560166</v>
       </c>
       <c r="D71">
-        <v>-0.058125823156614347</v>
+        <v>-0.057482324030135194</v>
       </c>
       <c r="E71">
-        <v>-0.037227908535724503</v>
+        <v>-0.036114413784102052</v>
       </c>
     </row>
     <row r="72">
@@ -1772,16 +1772,16 @@
         <v>75</v>
       </c>
       <c r="B72">
-        <v>-0.046194125529341393</v>
+        <v>-0.05614475647951412</v>
       </c>
       <c r="C72">
-        <v>0.018333627651664429</v>
+        <v>0.020108388112155332</v>
       </c>
       <c r="D72">
-        <v>-0.082127734734376526</v>
+        <v>-0.095556901246033416</v>
       </c>
       <c r="E72">
-        <v>-0.01026051632430626</v>
+        <v>-0.016732611712994817</v>
       </c>
     </row>
     <row r="73">
@@ -1789,16 +1789,16 @@
         <v>76</v>
       </c>
       <c r="B73">
-        <v>0.078739783975844302</v>
+        <v>0.085398960305385851</v>
       </c>
       <c r="C73">
-        <v>0.038336212676264886</v>
+        <v>0.039692023734831113</v>
       </c>
       <c r="D73">
-        <v>0.0036014365149175387</v>
+        <v>0.0076031779289928575</v>
       </c>
       <c r="E73">
-        <v>0.15387813143677107</v>
+        <v>0.16319474268177886</v>
       </c>
     </row>
     <row r="74">
@@ -1806,16 +1806,16 @@
         <v>77</v>
       </c>
       <c r="B74">
-        <v>-0.15923877077341891</v>
+        <v>-0.15945089947193036</v>
       </c>
       <c r="C74">
-        <v>0.0034562836545018174</v>
+        <v>0.0032787577214816433</v>
       </c>
       <c r="D74">
-        <v>-0.16601297436961976</v>
+        <v>-0.16587715920671051</v>
       </c>
       <c r="E74">
-        <v>-0.15246456717721807</v>
+        <v>-0.15302463973715022</v>
       </c>
     </row>
     <row r="75">
@@ -1823,16 +1823,16 @@
         <v>78</v>
       </c>
       <c r="B75">
-        <v>-0.0018651402269305685</v>
+        <v>-0.0030666712268100815</v>
       </c>
       <c r="C75">
-        <v>0.0073950040732087855</v>
+        <v>0.0067321408505198908</v>
       </c>
       <c r="D75">
-        <v>-0.016359107792758596</v>
+        <v>-0.016261450881652831</v>
       </c>
       <c r="E75">
-        <v>0.012628827338897457</v>
+        <v>0.010128108428032667</v>
       </c>
     </row>
     <row r="76">
@@ -1840,16 +1840,16 @@
         <v>79</v>
       </c>
       <c r="B76">
-        <v>-0.007414839894582954</v>
+        <v>-0.010316421147040997</v>
       </c>
       <c r="C76">
-        <v>0.016633209205159066</v>
+        <v>0.015307127031262194</v>
       </c>
       <c r="D76">
-        <v>-0.040015389177390788</v>
+        <v>-0.040317898063643887</v>
       </c>
       <c r="E76">
-        <v>0.025185709388224876</v>
+        <v>0.019685055769561897</v>
       </c>
     </row>
     <row r="77">
@@ -1857,16 +1857,16 @@
         <v>80</v>
       </c>
       <c r="B77">
-        <v>-0.083410216172623203</v>
+        <v>-0.084444356126472345</v>
       </c>
       <c r="C77">
-        <v>0.0029315670592945462</v>
+        <v>0.0025265715385520146</v>
       </c>
       <c r="D77">
-        <v>-0.089155992197363754</v>
+        <v>-0.089396355044024392</v>
       </c>
       <c r="E77">
-        <v>-0.077664440147882652</v>
+        <v>-0.079492357208920297</v>
       </c>
     </row>
     <row r="78">
@@ -1874,16 +1874,16 @@
         <v>81</v>
       </c>
       <c r="B78">
-        <v>-0.062869711096339626</v>
+        <v>-0.067474666016984028</v>
       </c>
       <c r="C78">
-        <v>0.0070502796245107734</v>
+        <v>0.0083518980513263025</v>
       </c>
       <c r="D78">
-        <v>-0.076688029700308052</v>
+        <v>-0.08384411745684929</v>
       </c>
       <c r="E78">
-        <v>-0.049051392492371206</v>
+        <v>-0.051105214577118765</v>
       </c>
     </row>
     <row r="79">
@@ -1891,16 +1891,16 @@
         <v>82</v>
       </c>
       <c r="B79">
-        <v>-0.017532873095500608</v>
+        <v>-0.01432732953841555</v>
       </c>
       <c r="C79">
-        <v>0.014790991259070197</v>
+        <v>0.014570834037824857</v>
       </c>
       <c r="D79">
-        <v>-0.046522734572168864</v>
+        <v>-0.042885695403840927</v>
       </c>
       <c r="E79">
-        <v>0.011456988381167647</v>
+        <v>0.01423103632700983</v>
       </c>
     </row>
     <row r="80">
@@ -1908,16 +1908,16 @@
         <v>83</v>
       </c>
       <c r="B80">
-        <v>-0.18505592351880421</v>
+        <v>-0.18402558909233371</v>
       </c>
       <c r="C80">
-        <v>0.0042937063687695362</v>
+        <v>0.0042581296014338691</v>
       </c>
       <c r="D80">
-        <v>-0.19347145263606189</v>
+        <v>-0.19237139099496164</v>
       </c>
       <c r="E80">
-        <v>-0.17664039440154652</v>
+        <v>-0.17567978718970578</v>
       </c>
     </row>
     <row r="81">
@@ -1925,16 +1925,16 @@
         <v>84</v>
       </c>
       <c r="B81">
-        <v>-0.018308403510444618</v>
+        <v>-0.022096456045802359</v>
       </c>
       <c r="C81">
-        <v>0.0085069945723580554</v>
+        <v>0.0093681023042619001</v>
       </c>
       <c r="D81">
-        <v>-0.034981844676508431</v>
+        <v>-0.040457645899815847</v>
       </c>
       <c r="E81">
-        <v>-0.0016349623443808088</v>
+        <v>-0.0037352661917888705</v>
       </c>
     </row>
     <row r="82">
@@ -1942,16 +1942,16 @@
         <v>85</v>
       </c>
       <c r="B82">
-        <v>-0.0071812549781108776</v>
+        <v>-0.0090770769858201806</v>
       </c>
       <c r="C82">
-        <v>0.018949122299557176</v>
+        <v>0.018895224350190951</v>
       </c>
       <c r="D82">
-        <v>-0.04432093728575303</v>
+        <v>-0.046111130453639293</v>
       </c>
       <c r="E82">
-        <v>0.029958427329531277</v>
+        <v>0.027956976481998935</v>
       </c>
     </row>
     <row r="83">
@@ -1959,16 +1959,16 @@
         <v>86</v>
       </c>
       <c r="B83">
-        <v>-0.10901405562204652</v>
+        <v>-0.11007111346813797</v>
       </c>
       <c r="C83">
-        <v>0.0033574388781529834</v>
+        <v>0.0033266266163986527</v>
       </c>
       <c r="D83">
-        <v>-0.11559452909030474</v>
+        <v>-0.11659119744054768</v>
       </c>
       <c r="E83">
-        <v>-0.10243358215378831</v>
+        <v>-0.10355102949572827</v>
       </c>
     </row>
     <row r="84">
@@ -1976,16 +1976,16 @@
         <v>87</v>
       </c>
       <c r="B84">
-        <v>-0.07222465978151929</v>
+        <v>-0.076692678080882773</v>
       </c>
       <c r="C84">
-        <v>0.0075233826200274152</v>
+        <v>0.0071685905447754919</v>
       </c>
       <c r="D84">
-        <v>-0.086970250548574671</v>
+        <v>-0.090742891015918481</v>
       </c>
       <c r="E84">
-        <v>-0.05747906901446391</v>
+        <v>-0.062642465145847065</v>
       </c>
     </row>
     <row r="85">
@@ -1993,16 +1993,16 @@
         <v>88</v>
       </c>
       <c r="B85">
-        <v>-0.026287899388465676</v>
+        <v>-0.022822181626372298</v>
       </c>
       <c r="C85">
-        <v>0.01562419681434111</v>
+        <v>0.01554412521106651</v>
       </c>
       <c r="D85">
-        <v>-0.056910828451638168</v>
+        <v>-0.053288180171025018</v>
       </c>
       <c r="E85">
-        <v>0.0043350296747068154</v>
+        <v>0.0076438169182804182</v>
       </c>
     </row>
     <row r="86">
@@ -2010,16 +2010,16 @@
         <v>89</v>
       </c>
       <c r="B86">
-        <v>-0.11371819508492412</v>
+        <v>-0.1137960846818187</v>
       </c>
       <c r="C86">
-        <v>0.0043625538665381727</v>
+        <v>0.0041192415283137131</v>
       </c>
       <c r="D86">
-        <v>-0.12226871385705573</v>
+        <v>-0.12186972137083646</v>
       </c>
       <c r="E86">
-        <v>-0.1051676763127925</v>
+        <v>-0.10572244799280095</v>
       </c>
     </row>
     <row r="87">
@@ -2027,16 +2027,16 @@
         <v>90</v>
       </c>
       <c r="B87">
-        <v>-0.029773817137353102</v>
+        <v>-0.029790481376462768</v>
       </c>
       <c r="C87">
-        <v>0.013152558784098203</v>
+        <v>0.013194536739621737</v>
       </c>
       <c r="D87">
-        <v>-0.055552570644009008</v>
+        <v>-0.055651527683988178</v>
       </c>
       <c r="E87">
-        <v>-0.0039950636306971994</v>
+        <v>-0.0039294350689373543</v>
       </c>
     </row>
     <row r="88">
@@ -2044,16 +2044,16 @@
         <v>91</v>
       </c>
       <c r="B88">
-        <v>-0.012673999062524945</v>
+        <v>-0.011311984915211657</v>
       </c>
       <c r="C88">
-        <v>0.029473057012982213</v>
+        <v>0.028115502038136227</v>
       </c>
       <c r="D88">
-        <v>-0.070440604351822519</v>
+        <v>-0.066417845356994062</v>
       </c>
       <c r="E88">
-        <v>0.045092606226772636</v>
+        <v>0.043793875526570755</v>
       </c>
     </row>
     <row r="89">
@@ -2061,16 +2061,16 @@
         <v>92</v>
       </c>
       <c r="B89">
-        <v>-0.051178024054218459</v>
+        <v>-0.051995259843069207</v>
       </c>
       <c r="C89">
-        <v>0.0051611545875204995</v>
+        <v>0.0054792317358581984</v>
       </c>
       <c r="D89">
-        <v>-0.061293802312532709</v>
+        <v>-0.062734473407999924</v>
       </c>
       <c r="E89">
-        <v>-0.041062245795904208</v>
+        <v>-0.041256046278138489</v>
       </c>
     </row>
     <row r="90">
@@ -2078,16 +2078,16 @@
         <v>93</v>
       </c>
       <c r="B90">
-        <v>-0.087465197644080409</v>
+        <v>-0.093957573264244768</v>
       </c>
       <c r="C90">
-        <v>0.017866640615705077</v>
+        <v>0.017778873606432766</v>
       </c>
       <c r="D90">
-        <v>-0.12248351992539221</v>
+        <v>-0.12880390388279936</v>
       </c>
       <c r="E90">
-        <v>-0.052446875362768611</v>
+        <v>-0.059111242645690183</v>
       </c>
     </row>
     <row r="91">
@@ -2095,16 +2095,16 @@
         <v>94</v>
       </c>
       <c r="B91">
-        <v>0.069831253333309681</v>
+        <v>0.074905786695419932</v>
       </c>
       <c r="C91">
-        <v>0.033563537776673244</v>
+        <v>0.032340813343697213</v>
       </c>
       <c r="D91">
-        <v>0.0040472703202196619</v>
+        <v>0.011518268498559719</v>
       </c>
       <c r="E91">
-        <v>0.13561523634639971</v>
+        <v>0.13829330489228014</v>
       </c>
     </row>
     <row r="92">
@@ -2112,16 +2112,16 @@
         <v>95</v>
       </c>
       <c r="B92">
-        <v>-0.14196096543693368</v>
+        <v>-0.14281461193191233</v>
       </c>
       <c r="C92">
-        <v>0.0032169626706329744</v>
+        <v>0.0032747694121173267</v>
       </c>
       <c r="D92">
-        <v>-0.14826610768527351</v>
+        <v>-0.14923305470854709</v>
       </c>
       <c r="E92">
-        <v>-0.13565582318859384</v>
+        <v>-0.13639616915527758</v>
       </c>
     </row>
     <row r="93">
@@ -2129,16 +2129,16 @@
         <v>96</v>
       </c>
       <c r="B93">
-        <v>-0.005003391378839009</v>
+        <v>-0.012468013944203689</v>
       </c>
       <c r="C93">
-        <v>0.0069219677770610468</v>
+        <v>0.0072294890991343426</v>
       </c>
       <c r="D93">
-        <v>-0.018570223183016297</v>
+        <v>-0.026637580178516598</v>
       </c>
       <c r="E93">
-        <v>0.008563440425338277</v>
+        <v>0.0017015522901092216</v>
       </c>
     </row>
     <row r="94">
@@ -2146,16 +2146,16 @@
         <v>97</v>
       </c>
       <c r="B94">
-        <v>0.041324969437119281</v>
+        <v>0.043161158771894033</v>
       </c>
       <c r="C94">
-        <v>0.015150369218827568</v>
+        <v>0.013971691432195329</v>
       </c>
       <c r="D94">
-        <v>0.01163073831917432</v>
+        <v>0.015777092700395404</v>
       </c>
       <c r="E94">
-        <v>0.071019200555064249</v>
+        <v>0.070545224843392665</v>
       </c>
     </row>
     <row r="95">
@@ -2163,16 +2163,16 @@
         <v>98</v>
       </c>
       <c r="B95">
-        <v>-0.081678425340977051</v>
+        <v>-0.080995696548978646</v>
       </c>
       <c r="C95">
-        <v>0.0030243059994102348</v>
+        <v>0.003139346262878465</v>
       </c>
       <c r="D95">
-        <v>-0.087605966670040808</v>
+        <v>-0.087148714208832717</v>
       </c>
       <c r="E95">
-        <v>-0.075750884011913294</v>
+        <v>-0.074842678889124575</v>
       </c>
     </row>
     <row r="96">
@@ -2180,16 +2180,16 @@
         <v>99</v>
       </c>
       <c r="B96">
-        <v>-0.059376856823707323</v>
+        <v>-0.060327024338348814</v>
       </c>
       <c r="C96">
-        <v>0.0071919659232570392</v>
+        <v>0.0070479546383739921</v>
       </c>
       <c r="D96">
-        <v>-0.073472875961862541</v>
+        <v>-0.074140788646081826</v>
       </c>
       <c r="E96">
-        <v>-0.045280837685552106</v>
+        <v>-0.046513260030615802</v>
       </c>
     </row>
     <row r="97">
@@ -2197,16 +2197,16 @@
         <v>100</v>
       </c>
       <c r="B97">
-        <v>0.002994153137525114</v>
+        <v>0.0062358317574272232</v>
       </c>
       <c r="C97">
-        <v>0.014450742464973663</v>
+        <v>0.015249413004536493</v>
       </c>
       <c r="D97">
-        <v>-0.025328831776531884</v>
+        <v>-0.023652527047978558</v>
       </c>
       <c r="E97">
-        <v>0.031317138051582108</v>
+        <v>0.036124190562833003</v>
       </c>
     </row>
     <row r="98">
@@ -2214,16 +2214,16 @@
         <v>101</v>
       </c>
       <c r="B98">
-        <v>-0.16946180464492944</v>
+        <v>-0.16781806869445853</v>
       </c>
       <c r="C98">
-        <v>0.004183182317289637</v>
+        <v>0.0040427532631744862</v>
       </c>
       <c r="D98">
-        <v>-0.17766071010572296</v>
+        <v>-0.17574173965653903</v>
       </c>
       <c r="E98">
-        <v>-0.16126289918413592</v>
+        <v>-0.15989439773237804</v>
       </c>
     </row>
     <row r="99">
@@ -2231,16 +2231,16 @@
         <v>102</v>
       </c>
       <c r="B99">
-        <v>-0.0060947268745438548</v>
+        <v>-0.010393350611992034</v>
       </c>
       <c r="C99">
-        <v>0.0083895599087353695</v>
+        <v>0.008888208107363715</v>
       </c>
       <c r="D99">
-        <v>-0.022537999802211033</v>
+        <v>-0.027813962729671633</v>
       </c>
       <c r="E99">
-        <v>0.010348546053123322</v>
+        <v>0.0070272615056875664</v>
       </c>
     </row>
     <row r="100">
@@ -2248,16 +2248,16 @@
         <v>103</v>
       </c>
       <c r="B100">
-        <v>0.041025135014548089</v>
+        <v>0.048032717617715714</v>
       </c>
       <c r="C100">
-        <v>0.01830260210605195</v>
+        <v>0.01762359913009617</v>
       </c>
       <c r="D100">
-        <v>0.0051526119036577819</v>
+        <v>0.013491010126806972</v>
       </c>
       <c r="E100">
-        <v>0.07689765812543839</v>
+        <v>0.08257442510862445</v>
       </c>
     </row>
     <row r="101">
@@ -2265,16 +2265,16 @@
         <v>104</v>
       </c>
       <c r="B101">
-        <v>-0.11019916749085472</v>
+        <v>-0.11044184695718932</v>
       </c>
       <c r="C101">
-        <v>0.0034874953859039509</v>
+        <v>0.0038436582799995051</v>
       </c>
       <c r="D101">
-        <v>-0.11703454757981079</v>
+        <v>-0.11797529679592572</v>
       </c>
       <c r="E101">
-        <v>-0.10336378740189865</v>
+        <v>-0.10290839711845293</v>
       </c>
     </row>
     <row r="102">
@@ -2282,16 +2282,16 @@
         <v>105</v>
       </c>
       <c r="B102">
-        <v>-0.068041519176678861</v>
+        <v>-0.071197008764539244</v>
       </c>
       <c r="C102">
-        <v>0.0077762346280091446</v>
+        <v>0.0077558841421692514</v>
       </c>
       <c r="D102">
-        <v>-0.083282691841217643</v>
+        <v>-0.086398298755409775</v>
       </c>
       <c r="E102">
-        <v>-0.052800346512140085</v>
+        <v>-0.055995718773668719</v>
       </c>
     </row>
     <row r="103">
@@ -2299,16 +2299,16 @@
         <v>106</v>
       </c>
       <c r="B103">
-        <v>0.0053048411600367038</v>
+        <v>0.010473269884189553</v>
       </c>
       <c r="C103">
-        <v>0.015718151838548557</v>
+        <v>0.015296487759546893</v>
       </c>
       <c r="D103">
-        <v>-0.025502236763753849</v>
+        <v>-0.019507367011920414</v>
       </c>
       <c r="E103">
-        <v>0.036111919083827257</v>
+        <v>0.040453906780299524</v>
       </c>
     </row>
     <row r="104">
@@ -2316,16 +2316,16 @@
         <v>107</v>
       </c>
       <c r="B104">
-        <v>-0.10414532973901802</v>
+        <v>-0.10408330759587216</v>
       </c>
       <c r="C104">
-        <v>0.004121521747591529</v>
+        <v>0.0042391013200833248</v>
       </c>
       <c r="D104">
-        <v>-0.11222343035408161</v>
+        <v>-0.11239186724478863</v>
       </c>
       <c r="E104">
-        <v>-0.096067229123954434</v>
+        <v>-0.095774747946955688</v>
       </c>
     </row>
     <row r="105">
@@ -2333,16 +2333,16 @@
         <v>108</v>
       </c>
       <c r="B105">
-        <v>-0.046212112647714243</v>
+        <v>-0.051106127416366033</v>
       </c>
       <c r="C105">
-        <v>0.012557322932435328</v>
+        <v>0.01231669666863869</v>
       </c>
       <c r="D105">
-        <v>-0.070824215729139314</v>
+        <v>-0.075246623531468035</v>
       </c>
       <c r="E105">
-        <v>-0.021600009566289168</v>
+        <v>-0.026965631301264035</v>
       </c>
     </row>
     <row r="106">
@@ -2350,16 +2350,16 @@
         <v>109</v>
       </c>
       <c r="B106">
-        <v>-0.037619693573605971</v>
+        <v>-0.05244307518419751</v>
       </c>
       <c r="C106">
-        <v>0.026146841580551687</v>
+        <v>0.029057997637955326</v>
       </c>
       <c r="D106">
-        <v>-0.088866982800516497</v>
+        <v>-0.10939620945093873</v>
       </c>
       <c r="E106">
-        <v>0.013627595653304549</v>
+        <v>0.0045100590825437117</v>
       </c>
     </row>
     <row r="107">
@@ -2367,16 +2367,16 @@
         <v>110</v>
       </c>
       <c r="B107">
-        <v>-0.050372057225798954</v>
+        <v>-0.049592685558382678</v>
       </c>
       <c r="C107">
-        <v>0.0051351437840477182</v>
+        <v>0.004993440528524345</v>
       </c>
       <c r="D107">
-        <v>-0.060436854736338766</v>
+        <v>-0.05937975550628373</v>
       </c>
       <c r="E107">
-        <v>-0.040307259715259142</v>
+        <v>-0.039805615610481626</v>
       </c>
     </row>
     <row r="108">
@@ -2384,16 +2384,16 @@
         <v>111</v>
       </c>
       <c r="B108">
-        <v>-0.097124801747366096</v>
+        <v>-0.1014437480393427</v>
       </c>
       <c r="C108">
-        <v>0.017462006339600725</v>
+        <v>0.017664854556745178</v>
       </c>
       <c r="D108">
-        <v>-0.13135004749059428</v>
+        <v>-0.13606660299851753</v>
       </c>
       <c r="E108">
-        <v>-0.062899556004137908</v>
+        <v>-0.066820893080167879</v>
       </c>
     </row>
     <row r="109">
@@ -2401,16 +2401,16 @@
         <v>112</v>
       </c>
       <c r="B109">
-        <v>0.11523130561465883</v>
+        <v>0.11124404080365762</v>
       </c>
       <c r="C109">
-        <v>0.032548841437370996</v>
+        <v>0.032050050150394138</v>
       </c>
       <c r="D109">
-        <v>0.051436110767829876</v>
+        <v>0.048426414186536149</v>
       </c>
       <c r="E109">
-        <v>0.17902650046148777</v>
+        <v>0.17406166742077908</v>
       </c>
     </row>
     <row r="110">
@@ -2418,16 +2418,16 @@
         <v>113</v>
       </c>
       <c r="B110">
-        <v>-0.14019731909919314</v>
+        <v>-0.13820462244421641</v>
       </c>
       <c r="C110">
-        <v>0.0032441069000600912</v>
+        <v>0.0034943296308344923</v>
       </c>
       <c r="D110">
-        <v>-0.1465556631547289</v>
+        <v>-0.14505339619152868</v>
       </c>
       <c r="E110">
-        <v>-0.13383897504365738</v>
+        <v>-0.13135584869690414</v>
       </c>
     </row>
     <row r="111">
@@ -2435,16 +2435,16 @@
         <v>114</v>
       </c>
       <c r="B111">
-        <v>-0.016591811528360742</v>
+        <v>-0.019637847557512481</v>
       </c>
       <c r="C111">
-        <v>0.0070724723828879789</v>
+        <v>0.0078875937550413732</v>
       </c>
       <c r="D111">
-        <v>-0.030453627466930366</v>
+        <v>-0.035097277761895002</v>
       </c>
       <c r="E111">
-        <v>-0.0027299955897911194</v>
+        <v>-0.0041784173531299613</v>
       </c>
     </row>
     <row r="112">
@@ -2452,16 +2452,16 @@
         <v>115</v>
       </c>
       <c r="B112">
-        <v>0.053380211717096324</v>
+        <v>0.052307772150244125</v>
       </c>
       <c r="C112">
-        <v>0.015064765145543656</v>
+        <v>0.014734549830723035</v>
       </c>
       <c r="D112">
-        <v>0.023853761799729038</v>
+        <v>0.023428528140565258</v>
       </c>
       <c r="E112">
-        <v>0.082906661634463613</v>
+        <v>0.081187016159922992</v>
       </c>
     </row>
     <row r="113">
@@ -2469,16 +2469,16 @@
         <v>116</v>
       </c>
       <c r="B113">
-        <v>-0.079322810351780487</v>
+        <v>-0.078416173945079812</v>
       </c>
       <c r="C113">
-        <v>0.0032207551414602203</v>
+        <v>0.0033212670083891589</v>
       </c>
       <c r="D113">
-        <v>-0.085635385605581857</v>
+        <v>-0.084925750412433748</v>
       </c>
       <c r="E113">
-        <v>-0.073010235097979118</v>
+        <v>-0.071906597477725875</v>
       </c>
     </row>
     <row r="114">
@@ -2486,16 +2486,16 @@
         <v>117</v>
       </c>
       <c r="B114">
-        <v>-0.057690653867224079</v>
+        <v>-0.056011427797482742</v>
       </c>
       <c r="C114">
-        <v>0.0075718372068546485</v>
+        <v>0.0081163606808937003</v>
       </c>
       <c r="D114">
-        <v>-0.072531208357849736</v>
+        <v>-0.071919233570234317</v>
       </c>
       <c r="E114">
-        <v>-0.042850099376598429</v>
+        <v>-0.040103622024731167</v>
       </c>
     </row>
     <row r="115">
@@ -2503,16 +2503,16 @@
         <v>118</v>
       </c>
       <c r="B115">
-        <v>0.023896240468594749</v>
+        <v>0.026573483201570831</v>
       </c>
       <c r="C115">
-        <v>0.014772677062427381</v>
+        <v>0.015692253513607039</v>
       </c>
       <c r="D115">
-        <v>-0.0050577257787117746</v>
+        <v>-0.0041828287522434546</v>
       </c>
       <c r="E115">
-        <v>0.052850206715901273</v>
+        <v>0.057329795155385117</v>
       </c>
     </row>
     <row r="116">
@@ -2520,16 +2520,16 @@
         <v>119</v>
       </c>
       <c r="B116">
-        <v>-0.16104206914809668</v>
+        <v>-0.15866658764778946</v>
       </c>
       <c r="C116">
-        <v>0.0042933382017036198</v>
+        <v>0.0044949724101494498</v>
       </c>
       <c r="D116">
-        <v>-0.1694568766695122</v>
+        <v>-0.16747659410702287</v>
       </c>
       <c r="E116">
-        <v>-0.15262726162668117</v>
+        <v>-0.14985658118855605</v>
       </c>
     </row>
     <row r="117">
@@ -2537,16 +2537,16 @@
         <v>120</v>
       </c>
       <c r="B117">
-        <v>-0.00012339052983657451</v>
+        <v>0.0018800750460841967</v>
       </c>
       <c r="C117">
-        <v>0.0087745415793281205</v>
+        <v>0.0084868092483118968</v>
       </c>
       <c r="D117">
-        <v>-0.017321215394741199</v>
+        <v>-0.014753807761980386</v>
       </c>
       <c r="E117">
-        <v>0.017074434335068049</v>
+        <v>0.018513957854148781</v>
       </c>
     </row>
     <row r="118">
@@ -2554,16 +2554,16 @@
         <v>121</v>
       </c>
       <c r="B118">
-        <v>0.082939820288388408</v>
+        <v>0.085224311246080778</v>
       </c>
       <c r="C118">
-        <v>0.019015532198824351</v>
+        <v>0.015451433070660299</v>
       </c>
       <c r="D118">
-        <v>0.045669976671854226</v>
+        <v>0.054939981836280509</v>
       </c>
       <c r="E118">
-        <v>0.12020966390492259</v>
+        <v>0.11550864065588104</v>
       </c>
     </row>
     <row r="119">
@@ -2571,16 +2571,16 @@
         <v>122</v>
       </c>
       <c r="B119">
-        <v>-0.10872298518929989</v>
+        <v>-0.10778401527859761</v>
       </c>
       <c r="C119">
-        <v>0.0037601770801152347</v>
+        <v>0.0040222180548730429</v>
       </c>
       <c r="D119">
-        <v>-0.11609281273036391</v>
+        <v>-0.11566743668328341</v>
       </c>
       <c r="E119">
-        <v>-0.10135315764823587</v>
+        <v>-0.099900593873911814</v>
       </c>
     </row>
     <row r="120">
@@ -2588,16 +2588,16 @@
         <v>123</v>
       </c>
       <c r="B120">
-        <v>-0.050077851708059187</v>
+        <v>-0.051719826742691655</v>
       </c>
       <c r="C120">
-        <v>0.0083705827184052135</v>
+        <v>0.0099290231683988091</v>
       </c>
       <c r="D120">
-        <v>-0.066483927735459136</v>
+        <v>-0.071180401158478054</v>
       </c>
       <c r="E120">
-        <v>-0.033671775680659238</v>
+        <v>-0.032259252326905255</v>
       </c>
     </row>
     <row r="121">
@@ -2605,16 +2605,16 @@
         <v>124</v>
       </c>
       <c r="B121">
-        <v>0.0040104904996270674</v>
+        <v>0.0053170763939377587</v>
       </c>
       <c r="C121">
-        <v>0.016333834731802676</v>
+        <v>0.016760492089062037</v>
       </c>
       <c r="D121">
-        <v>-0.028003306322393444</v>
+        <v>-0.027532963132859935</v>
       </c>
       <c r="E121">
-        <v>0.036024287321647579</v>
+        <v>0.038167115920735455</v>
       </c>
     </row>
     <row r="122">
@@ -2622,16 +2622,16 @@
         <v>125</v>
       </c>
       <c r="B122">
-        <v>-0.10825635717395427</v>
+        <v>-0.10709765727838357</v>
       </c>
       <c r="C122">
-        <v>0.0043225201518116195</v>
+        <v>0.0044921496396443618</v>
       </c>
       <c r="D122">
-        <v>-0.1167284106618144</v>
+        <v>-0.11590218692149909</v>
       </c>
       <c r="E122">
-        <v>-0.099784303686094131</v>
+        <v>-0.098293127635268041</v>
       </c>
     </row>
     <row r="123">
@@ -2639,16 +2639,16 @@
         <v>126</v>
       </c>
       <c r="B123">
-        <v>-0.066608121099059725</v>
+        <v>-0.064382951476683437</v>
       </c>
       <c r="C123">
-        <v>0.013206716257272587</v>
+        <v>0.013142607619872388</v>
       </c>
       <c r="D123">
-        <v>-0.092493022175509698</v>
+        <v>-0.090142217676498493</v>
       </c>
       <c r="E123">
-        <v>-0.040723220022609745</v>
+        <v>-0.03862368527686838</v>
       </c>
     </row>
     <row r="124">
@@ -2656,16 +2656,16 @@
         <v>127</v>
       </c>
       <c r="B124">
-        <v>-0.019061748960990423</v>
+        <v>-0.015513450222976661</v>
       </c>
       <c r="C124">
-        <v>0.026397353551652021</v>
+        <v>0.022338701136472346</v>
       </c>
       <c r="D124">
-        <v>-0.070800036666559693</v>
+        <v>-0.059296888470225316</v>
       </c>
       <c r="E124">
-        <v>0.032676538744578848</v>
+        <v>0.02826998802427199</v>
       </c>
     </row>
     <row r="125">
@@ -2673,16 +2673,16 @@
         <v>128</v>
       </c>
       <c r="B125">
-        <v>-0.053979158149525433</v>
+        <v>-0.053853946973248544</v>
       </c>
       <c r="C125">
-        <v>0.0052633938764175062</v>
+        <v>0.006176283394392898</v>
       </c>
       <c r="D125">
-        <v>-0.064295323735564874</v>
+        <v>-0.065959371530461899</v>
       </c>
       <c r="E125">
-        <v>-0.043662992563485992</v>
+        <v>-0.041748522416035196</v>
       </c>
     </row>
     <row r="126">
@@ -2690,16 +2690,16 @@
         <v>129</v>
       </c>
       <c r="B126">
-        <v>-0.10862811582496279</v>
+        <v>-0.11634486578352096</v>
       </c>
       <c r="C126">
-        <v>0.017649134857501032</v>
+        <v>0.016672608682655753</v>
       </c>
       <c r="D126">
-        <v>-0.14322013039109421</v>
+        <v>-0.1490229334322721</v>
       </c>
       <c r="E126">
-        <v>-0.07403610125883138</v>
+        <v>-0.083666798134769821</v>
       </c>
     </row>
     <row r="127">
@@ -2707,16 +2707,16 @@
         <v>130</v>
       </c>
       <c r="B127">
-        <v>0.12194505096410893</v>
+        <v>0.12348714347297432</v>
       </c>
       <c r="C127">
-        <v>0.032239825914592138</v>
+        <v>0.028197948076365591</v>
       </c>
       <c r="D127">
-        <v>0.058755521468665958</v>
+        <v>0.068219580229915588</v>
       </c>
       <c r="E127">
-        <v>0.18513458045955189</v>
+        <v>0.17875470671603305</v>
       </c>
     </row>
     <row r="128">
@@ -2724,16 +2724,16 @@
         <v>131</v>
       </c>
       <c r="B128">
-        <v>-0.13006744453323688</v>
+        <v>-0.12763386367672108</v>
       </c>
       <c r="C128">
-        <v>0.0034054306287694376</v>
+        <v>0.0033059457427795061</v>
       </c>
       <c r="D128">
-        <v>-0.13674197785227593</v>
+        <v>-0.13411341105925578</v>
       </c>
       <c r="E128">
-        <v>-0.12339291121419782</v>
+        <v>-0.1211543162941864</v>
       </c>
     </row>
     <row r="129">
@@ -2741,16 +2741,16 @@
         <v>132</v>
       </c>
       <c r="B129">
-        <v>-0.01664271672575976</v>
+        <v>-0.016850898565553676</v>
       </c>
       <c r="C129">
-        <v>0.0075572722280165521</v>
+        <v>0.0078605044891670167</v>
       </c>
       <c r="D129">
-        <v>-0.031454724599539907</v>
+        <v>-0.03225723467963712</v>
       </c>
       <c r="E129">
-        <v>-0.0018307088519796087</v>
+        <v>-0.0014445624514702309</v>
       </c>
     </row>
     <row r="130">
@@ -2758,16 +2758,16 @@
         <v>133</v>
       </c>
       <c r="B130">
-        <v>0.072803923968654441</v>
+        <v>0.073297670831290199</v>
       </c>
       <c r="C130">
-        <v>0.01571121843278759</v>
+        <v>0.015811939542865288</v>
       </c>
       <c r="D130">
-        <v>0.042010446625016809</v>
+        <v>0.042306777619706464</v>
       </c>
       <c r="E130">
-        <v>0.10359740131229207</v>
+        <v>0.10428856404287393</v>
       </c>
     </row>
     <row r="131">
@@ -2775,16 +2775,16 @@
         <v>134</v>
       </c>
       <c r="B131">
-        <v>-0.074574463435454888</v>
+        <v>-0.073630233841394416</v>
       </c>
       <c r="C131">
-        <v>0.0033988359716806355</v>
+        <v>0.003640982046867307</v>
       </c>
       <c r="D131">
-        <v>-0.081236071320627337</v>
+        <v>-0.080766441496629246</v>
       </c>
       <c r="E131">
-        <v>-0.067912855550282439</v>
+        <v>-0.066494026186159585</v>
       </c>
     </row>
     <row r="132">
@@ -2792,16 +2792,16 @@
         <v>135</v>
       </c>
       <c r="B132">
-        <v>-0.053692343598939873</v>
+        <v>-0.056039403972488015</v>
       </c>
       <c r="C132">
-        <v>0.0079391249793860242</v>
+        <v>0.0081945063931549728</v>
       </c>
       <c r="D132">
-        <v>-0.069252770169892064</v>
+        <v>-0.072100372826761086</v>
       </c>
       <c r="E132">
-        <v>-0.038131917027987676</v>
+        <v>-0.039978435118214944</v>
       </c>
     </row>
     <row r="133">
@@ -2809,16 +2809,16 @@
         <v>136</v>
       </c>
       <c r="B133">
-        <v>0.027508505283183163</v>
+        <v>0.03118444952182305</v>
       </c>
       <c r="C133">
-        <v>0.014591930531050269</v>
+        <v>0.016212249798428526</v>
       </c>
       <c r="D133">
-        <v>-0.0010912036452436977</v>
+        <v>-0.00059103841821438532</v>
       </c>
       <c r="E133">
-        <v>0.056108214211610025</v>
+        <v>0.062959937461860488</v>
       </c>
     </row>
     <row r="134">
@@ -2826,16 +2826,16 @@
         <v>137</v>
       </c>
       <c r="B134">
-        <v>-0.14407510385341085</v>
+        <v>-0.14151592318182502</v>
       </c>
       <c r="C134">
-        <v>0.0044263780234254334</v>
+        <v>0.0046453422878930421</v>
       </c>
       <c r="D134">
-        <v>-0.15275066523112127</v>
+        <v>-0.15062064993593807</v>
       </c>
       <c r="E134">
-        <v>-0.13539954247570044</v>
+        <v>-0.13241119642771196</v>
       </c>
     </row>
     <row r="135">
@@ -2843,16 +2843,16 @@
         <v>138</v>
       </c>
       <c r="B135">
-        <v>-0.0085113914891099558</v>
+        <v>-0.0021200956703464409</v>
       </c>
       <c r="C135">
-        <v>0.009219410541603348</v>
+        <v>0.0090885627248345289</v>
       </c>
       <c r="D135">
-        <v>-0.026581145494913021</v>
+        <v>-0.019933396621903986</v>
       </c>
       <c r="E135">
-        <v>0.0095583625166931075</v>
+        <v>0.015693205281211105</v>
       </c>
     </row>
     <row r="136">
@@ -2860,16 +2860,16 @@
         <v>139</v>
       </c>
       <c r="B136">
-        <v>0.10518893807573544</v>
+        <v>0.10005362941309449</v>
       </c>
       <c r="C136">
-        <v>0.019574826438879193</v>
+        <v>0.020369914246596042</v>
       </c>
       <c r="D136">
-        <v>0.066822895381283207</v>
+        <v>0.060129229503246132</v>
       </c>
       <c r="E136">
-        <v>0.14355498077018769</v>
+        <v>0.13997802932294284</v>
       </c>
     </row>
     <row r="137">
@@ -2877,16 +2877,16 @@
         <v>140</v>
       </c>
       <c r="B137">
-        <v>-0.093724484682920731</v>
+        <v>-0.091985501249714538</v>
       </c>
       <c r="C137">
-        <v>0.0040978434528238204</v>
+        <v>0.0042711296154182999</v>
       </c>
       <c r="D137">
-        <v>-0.10175612758008566</v>
+        <v>-0.10035678151672604</v>
       </c>
       <c r="E137">
-        <v>-0.085692841785755799</v>
+        <v>-0.083614220982703033</v>
       </c>
     </row>
     <row r="138">
@@ -2894,16 +2894,16 @@
         <v>141</v>
       </c>
       <c r="B138">
-        <v>-0.040524999781275772</v>
+        <v>-0.043422868184238551</v>
       </c>
       <c r="C138">
-        <v>0.0090622585143349497</v>
+        <v>0.0095165645687120097</v>
       </c>
       <c r="D138">
-        <v>-0.058286738380336878</v>
+        <v>-0.062075036663559555</v>
       </c>
       <c r="E138">
-        <v>-0.022763261182214663</v>
+        <v>-0.024770699704917548</v>
       </c>
     </row>
     <row r="139">
@@ -2911,16 +2911,16 @@
         <v>142</v>
       </c>
       <c r="B139">
-        <v>0.0047483451410771406</v>
+        <v>0.0088553175904277203</v>
       </c>
       <c r="C139">
-        <v>0.016551193399569425</v>
+        <v>0.014696516383496505</v>
       </c>
       <c r="D139">
-        <v>-0.027691467759938051</v>
+        <v>-0.019949394200770521</v>
       </c>
       <c r="E139">
-        <v>0.037188158042092329</v>
+        <v>0.037660029381625958</v>
       </c>
     </row>
     <row r="140">
@@ -2928,16 +2928,16 @@
         <v>143</v>
       </c>
       <c r="B140">
-        <v>-0.10120315313045795</v>
+        <v>-0.099491185909045529</v>
       </c>
       <c r="C140">
-        <v>0.0047350847848178666</v>
+        <v>0.0040796977054181217</v>
       </c>
       <c r="D140">
-        <v>-0.11048382508978163</v>
+        <v>-0.10748731744155342</v>
       </c>
       <c r="E140">
-        <v>-0.091922481171134274</v>
+        <v>-0.091495054376537641</v>
       </c>
     </row>
     <row r="141">
@@ -2945,16 +2945,16 @@
         <v>144</v>
       </c>
       <c r="B141">
-        <v>-0.051543264407332298</v>
+        <v>-0.051165125356079366</v>
       </c>
       <c r="C141">
-        <v>0.014311354199566275</v>
+        <v>0.01535017928585581</v>
       </c>
       <c r="D141">
-        <v>-0.079593233870544941</v>
+        <v>-0.081251190912914897</v>
       </c>
       <c r="E141">
-        <v>-0.023493294944119655</v>
+        <v>-0.021079059799243838</v>
       </c>
     </row>
     <row r="142">
@@ -2962,16 +2962,16 @@
         <v>145</v>
       </c>
       <c r="B142">
-        <v>-0.0075104143964499484</v>
+        <v>-0.0063425676245544189</v>
       </c>
       <c r="C142">
-        <v>0.026950239517674331</v>
+        <v>0.024897365485630457</v>
       </c>
       <c r="D142">
-        <v>-0.060332347594074381</v>
+        <v>-0.055140940349971745</v>
       </c>
       <c r="E142">
-        <v>0.045311518801174483</v>
+        <v>0.042455805100862901</v>
       </c>
     </row>
     <row r="143">
@@ -2979,16 +2979,16 @@
         <v>146</v>
       </c>
       <c r="B143">
-        <v>-0.048707300611915361</v>
+        <v>-0.046146890201939995</v>
       </c>
       <c r="C143">
-        <v>0.0057703112215877032</v>
+        <v>0.0053005693590706142</v>
       </c>
       <c r="D143">
-        <v>-0.060017015872175769</v>
+        <v>-0.056535928137724879</v>
       </c>
       <c r="E143">
-        <v>-0.037397585351654952</v>
+        <v>-0.035757852266155112</v>
       </c>
     </row>
     <row r="144">
@@ -2996,16 +2996,16 @@
         <v>147</v>
       </c>
       <c r="B144">
-        <v>-0.10745079143232188</v>
+        <v>-0.10446080666912214</v>
       </c>
       <c r="C144">
-        <v>0.018231871112785639</v>
+        <v>0.019750707645751989</v>
       </c>
       <c r="D144">
-        <v>-0.14318495949174198</v>
+        <v>-0.14317190298544152</v>
       </c>
       <c r="E144">
-        <v>-0.071716623372901772</v>
+        <v>-0.065749710352802734</v>
       </c>
     </row>
     <row r="145">
@@ -3013,16 +3013,16 @@
         <v>148</v>
       </c>
       <c r="B145">
-        <v>0.1045553629543301</v>
+        <v>0.093943430713132228</v>
       </c>
       <c r="C145">
-        <v>0.032985911358985362</v>
+        <v>0.030856332170787142</v>
       </c>
       <c r="D145">
-        <v>0.039903518236729926</v>
+        <v>0.033465473768202365</v>
       </c>
       <c r="E145">
-        <v>0.16920720767193026</v>
+        <v>0.1544213876580621</v>
       </c>
     </row>
     <row r="146">
@@ -3030,16 +3030,16 @@
         <v>149</v>
       </c>
       <c r="B146">
-        <v>-0.11489489623474755</v>
+        <v>-0.11165233007760297</v>
       </c>
       <c r="C146">
-        <v>0.0038004913542287275</v>
+        <v>0.0040732157852355127</v>
       </c>
       <c r="D146">
-        <v>-0.12234373573193788</v>
+        <v>-0.11963570207860016</v>
       </c>
       <c r="E146">
-        <v>-0.10744605673755722</v>
+        <v>-0.10366895807660578</v>
       </c>
     </row>
     <row r="147">
@@ -3047,16 +3047,16 @@
         <v>150</v>
       </c>
       <c r="B147">
-        <v>-0.0048269095614369021</v>
+        <v>-0.0061654688022631131</v>
       </c>
       <c r="C147">
-        <v>0.008625644723162143</v>
+        <v>0.009510652195204479</v>
       </c>
       <c r="D147">
-        <v>-0.021732892792034379</v>
+        <v>-0.024806041374341507</v>
       </c>
       <c r="E147">
-        <v>0.012079073669160577</v>
+        <v>0.012475103769815279</v>
       </c>
     </row>
     <row r="148">
@@ -3064,16 +3064,16 @@
         <v>151</v>
       </c>
       <c r="B148">
-        <v>0.055841541130426872</v>
+        <v>0.056759813130316542</v>
       </c>
       <c r="C148">
-        <v>0.016312203832122483</v>
+        <v>0.017636755982943949</v>
       </c>
       <c r="D148">
-        <v>0.023870151942622195</v>
+        <v>0.022192338356938381</v>
       </c>
       <c r="E148">
-        <v>0.08781293031823155</v>
+        <v>0.091327287903694709</v>
       </c>
     </row>
     <row r="149">
@@ -3081,16 +3081,16 @@
         <v>152</v>
       </c>
       <c r="B149">
-        <v>-0.067338399826298773</v>
+        <v>-0.064936279685255435</v>
       </c>
       <c r="C149">
-        <v>0.0042292397067911994</v>
+        <v>0.0036095670192559082</v>
       </c>
       <c r="D149">
-        <v>-0.075627572005771027</v>
+        <v>-0.072010914897219697</v>
       </c>
       <c r="E149">
-        <v>-0.059049227646826519</v>
+        <v>-0.057861644473291174</v>
       </c>
     </row>
     <row r="150">
@@ -3098,16 +3098,16 @@
         <v>153</v>
       </c>
       <c r="B150">
-        <v>-0.040857663150735593</v>
+        <v>-0.040693242705635881</v>
       </c>
       <c r="C150">
-        <v>0.0094594575416627833</v>
+        <v>0.0095120338801265303</v>
       </c>
       <c r="D150">
-        <v>-0.059397892062646104</v>
+        <v>-0.059336523040021391</v>
       </c>
       <c r="E150">
-        <v>-0.022317434238825082</v>
+        <v>-0.022049962371250367</v>
       </c>
     </row>
     <row r="151">
@@ -3115,16 +3115,16 @@
         <v>154</v>
       </c>
       <c r="B151">
-        <v>0.049170558203128031</v>
+        <v>0.052723759379233293</v>
       </c>
       <c r="C151">
-        <v>0.017685707177061714</v>
+        <v>0.017112100741044557</v>
       </c>
       <c r="D151">
-        <v>0.014507147739307176</v>
+        <v>0.01918459254635653</v>
       </c>
       <c r="E151">
-        <v>0.083833968666948894</v>
+        <v>0.086262926212110055</v>
       </c>
     </row>
     <row r="152">
@@ -3132,16 +3132,16 @@
         <v>155</v>
       </c>
       <c r="B152">
-        <v>-0.11835469438008221</v>
+        <v>-0.11441970327524904</v>
       </c>
       <c r="C152">
-        <v>0.0045402655611974088</v>
+        <v>0.0042322044165230199</v>
       </c>
       <c r="D152">
-        <v>-0.12725347174135035</v>
+        <v>-0.12271469261982752</v>
       </c>
       <c r="E152">
-        <v>-0.10945591701881409</v>
+        <v>-0.10612471393067056</v>
       </c>
     </row>
     <row r="153">
@@ -3149,16 +3149,16 @@
         <v>156</v>
       </c>
       <c r="B153">
-        <v>-0.0043655071424063925</v>
+        <v>0.0013242845275963722</v>
       </c>
       <c r="C153">
-        <v>0.0096029371307812649</v>
+        <v>0.0088035723099607766</v>
       </c>
       <c r="D153">
-        <v>-0.023186961171747449</v>
+        <v>-0.015930444053152363</v>
       </c>
       <c r="E153">
-        <v>0.014455946886934662</v>
+        <v>0.018579013108345106</v>
       </c>
     </row>
     <row r="154">
@@ -3166,16 +3166,16 @@
         <v>157</v>
       </c>
       <c r="B154">
-        <v>0.071705768472411419</v>
+        <v>0.070199494133705645</v>
       </c>
       <c r="C154">
-        <v>0.017981821285259384</v>
+        <v>0.018327665030653213</v>
       </c>
       <c r="D154">
-        <v>0.036461965657178234</v>
+        <v>0.034277839322624744</v>
       </c>
       <c r="E154">
-        <v>0.1069495712876446</v>
+        <v>0.10612114894478655</v>
       </c>
     </row>
     <row r="155">
@@ -3183,16 +3183,16 @@
         <v>158</v>
       </c>
       <c r="B155">
-        <v>-0.079113030640312818</v>
+        <v>-0.079313541912189089</v>
       </c>
       <c r="C155">
-        <v>0.0050690721311860629</v>
+        <v>0.0049992918353894298</v>
       </c>
       <c r="D155">
-        <v>-0.089048250871725507</v>
+        <v>-0.089111997323036776</v>
       </c>
       <c r="E155">
-        <v>-0.069177810408900128</v>
+        <v>-0.069515086501341403</v>
       </c>
     </row>
     <row r="156">
@@ -3200,16 +3200,16 @@
         <v>159</v>
       </c>
       <c r="B156">
-        <v>-0.030961987225322472</v>
+        <v>-0.031311275153978184</v>
       </c>
       <c r="C156">
-        <v>0.0109201120717866</v>
+        <v>0.010780248755668709</v>
       </c>
       <c r="D156">
-        <v>-0.052365059735857596</v>
+        <v>-0.052440225058947645</v>
       </c>
       <c r="E156">
-        <v>-0.0095589147147873491</v>
+        <v>-0.010182325249008722</v>
       </c>
     </row>
     <row r="157">
@@ -3217,16 +3217,16 @@
         <v>160</v>
       </c>
       <c r="B157">
-        <v>0.030657528896097686</v>
+        <v>0.035237670980132807</v>
       </c>
       <c r="C157">
-        <v>0.019861004021675035</v>
+        <v>0.016199009658989561</v>
       </c>
       <c r="D157">
-        <v>-0.0082694076054242796</v>
+        <v>0.0034881194296708662</v>
       </c>
       <c r="E157">
-        <v>0.069584465397619644</v>
+        <v>0.066987222530594748</v>
       </c>
     </row>
     <row r="158">
@@ -3234,16 +3234,16 @@
         <v>161</v>
       </c>
       <c r="B158">
-        <v>-0.099003506692090668</v>
+        <v>-0.096196902060140699</v>
       </c>
       <c r="C158">
-        <v>0.0061964850234941934</v>
+        <v>0.0063042066890334125</v>
       </c>
       <c r="D158">
-        <v>-0.11114849404021557</v>
+        <v>-0.10855302977682918</v>
       </c>
       <c r="E158">
-        <v>-0.086858519343965768</v>
+        <v>-0.083840774343452218</v>
       </c>
     </row>
     <row r="159">
@@ -3251,16 +3251,16 @@
         <v>162</v>
       </c>
       <c r="B159">
-        <v>-0.025167255195801985</v>
+        <v>-0.022466206509599636</v>
       </c>
       <c r="C159">
-        <v>0.017721306780108085</v>
+        <v>0.017614583680369878</v>
       </c>
       <c r="D159">
-        <v>-0.059900663865494454</v>
+        <v>-0.056990462513064756</v>
       </c>
       <c r="E159">
-        <v>0.0095661534738904833</v>
+        <v>0.012058049493865484</v>
       </c>
     </row>
     <row r="160">
@@ -3268,16 +3268,16 @@
         <v>163</v>
       </c>
       <c r="B160">
-        <v>0.021496595860758357</v>
+        <v>0.021188378296709203</v>
       </c>
       <c r="C160">
-        <v>0.035004804901065223</v>
+        <v>0.036783570367301212</v>
       </c>
       <c r="D160">
-        <v>-0.047112125218226122</v>
+        <v>-0.050906734657757968</v>
       </c>
       <c r="E160">
-        <v>0.090105316939742844</v>
+        <v>0.093283491251176381</v>
       </c>
     </row>
     <row r="161">
@@ -3285,16 +3285,16 @@
         <v>164</v>
       </c>
       <c r="B161">
-        <v>-0.050565763152233108</v>
+        <v>-0.048964814022214913</v>
       </c>
       <c r="C161">
-        <v>0.0073925592785875297</v>
+        <v>0.0074500390859931339</v>
       </c>
       <c r="D161">
-        <v>-0.065055057970964975</v>
+        <v>-0.063566780989218932</v>
       </c>
       <c r="E161">
-        <v>-0.036076468333501241</v>
+        <v>-0.034362847055210886</v>
       </c>
     </row>
     <row r="162">
@@ -3302,16 +3302,16 @@
         <v>165</v>
       </c>
       <c r="B162">
-        <v>-0.090421746790044069</v>
+        <v>-0.089493058656410898</v>
       </c>
       <c r="C162">
-        <v>0.021035706852529781</v>
+        <v>0.021039464053597565</v>
       </c>
       <c r="D162">
-        <v>-0.13165138686740546</v>
+        <v>-0.13073009856559767</v>
       </c>
       <c r="E162">
-        <v>-0.049192106712682676</v>
+        <v>-0.048256018747224128</v>
       </c>
     </row>
     <row r="163">
@@ -3319,16 +3319,16 @@
         <v>166</v>
       </c>
       <c r="B163">
-        <v>0.1516090631229754</v>
+        <v>0.15156082955758582</v>
       </c>
       <c r="C163">
-        <v>0.042136636530720334</v>
+        <v>0.040237948939316433</v>
       </c>
       <c r="D163">
-        <v>0.069021947300752867</v>
+        <v>0.072695041814732811</v>
       </c>
       <c r="E163">
-        <v>0.23419617894519792</v>
+        <v>0.23042661730043884</v>
       </c>
     </row>
   </sheetData>

</xml_diff>